<commit_message>
added non PID to temp sim
</commit_message>
<xml_diff>
--- a/Nichrome Wire Calculator.xlsx
+++ b/Nichrome Wire Calculator.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\obell\Documents\GitHub\TRACE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C204AF8C-BF87-4395-B662-F659A3B133CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5B821E-379F-4CED-8D61-DFDC50BF97BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{C209EC7C-6E6B-4133-B0CF-96CD40FF02C8}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Gauge(AWG)</t>
   </si>
@@ -126,16 +126,30 @@
   </si>
   <si>
     <t>Nichrome constants &amp; parameters</t>
+  </si>
+  <si>
+    <t>pink = selected size</t>
+  </si>
+  <si>
+    <t>green = initial posable size</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -170,30 +184,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -657,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EF71F9C-0B34-44D1-B309-BF9256BD69A8}">
   <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,10 +694,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="4"/>
+      <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -689,14 +706,14 @@
       <c r="B2" s="2">
         <v>1.1000000000000001E-6</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -709,12 +726,12 @@
       <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -727,12 +744,12 @@
       <c r="C4" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -744,26 +761,26 @@
       <c r="C5" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
       <c r="B6">
-        <v>220</v>
-      </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
+        <v>270</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -771,14 +788,14 @@
       </c>
       <c r="B7">
         <f>B6-B5</f>
-        <v>200</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
+        <v>250</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -790,12 +807,12 @@
       <c r="C8" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -810,18 +827,18 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="G14" s="4" t="s">
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="G14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -866,15 +883,15 @@
         <v>1.024</v>
       </c>
       <c r="C16">
-        <f>(PI()*(B16/1000/2)^2)</f>
+        <f t="shared" ref="C16:C28" si="0">(PI()*(B16/1000/2)^2)</f>
         <v>8.2354966458264271E-7</v>
       </c>
       <c r="D16">
-        <f>B16/1000*$B$8*PI()</f>
+        <f t="shared" ref="D16:D28" si="1">B16/1000*$B$8*PI()</f>
         <v>3.8603890527311377E-3</v>
       </c>
       <c r="E16">
-        <f>C16*$B$8</f>
+        <f t="shared" ref="E16:E28" si="2">C16*$B$8</f>
         <v>9.8825959749917113E-7</v>
       </c>
       <c r="F16">
@@ -886,20 +903,20 @@
         <v>1.3356814376913826</v>
       </c>
       <c r="H16">
-        <f>$B$9/(G16*$B$8)</f>
+        <f t="shared" ref="H16:H28" si="3">$B$9/(G16*$B$8)</f>
         <v>12.166074590425403</v>
       </c>
       <c r="I16">
-        <f>H16*$B$9</f>
+        <f t="shared" ref="I16:I28" si="4">H16*$B$9</f>
         <v>237.23845451329535</v>
       </c>
       <c r="J16">
-        <f>F16*$B$4*$B$7</f>
-        <v>763.72701694735952</v>
+        <f t="shared" ref="J16:J28" si="5">F16*$B$4*$B$7</f>
+        <v>954.6587711841994</v>
       </c>
       <c r="K16">
-        <f>J16/I16</f>
-        <v>3.2192378698224853</v>
+        <f t="shared" ref="K16:K28" si="6">J16/I16</f>
+        <v>4.0240473372781063</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -910,40 +927,40 @@
         <v>0.91</v>
       </c>
       <c r="C17">
-        <f>(PI()*(B17/1000/2)^2)</f>
+        <f t="shared" si="0"/>
         <v>6.503882191094269E-7</v>
       </c>
       <c r="D17">
-        <f>B17/1000*$B$8*PI()</f>
+        <f t="shared" si="1"/>
         <v>3.4306191777200537E-3</v>
       </c>
       <c r="E17">
-        <f>C17*$B$8</f>
+        <f t="shared" si="2"/>
         <v>7.8046586293131222E-7</v>
       </c>
       <c r="F17">
-        <f t="shared" ref="F17:F28" si="0">E17*$B$3</f>
+        <f t="shared" ref="F17:F28" si="7">E17*$B$3</f>
         <v>6.5559132486230224E-3</v>
       </c>
       <c r="G17" s="3">
-        <f>($B$2*1)/C17</f>
+        <f t="shared" ref="G16:G24" si="8">($B$2*1)/C17</f>
         <v>1.6912975476496548</v>
       </c>
       <c r="H17">
-        <f>$B$9/(G17*$B$8)</f>
+        <f t="shared" si="3"/>
         <v>9.608007782298353</v>
       </c>
       <c r="I17">
-        <f>H17*$B$9</f>
+        <f t="shared" si="4"/>
         <v>187.35615175481789</v>
       </c>
       <c r="J17">
-        <f>F17*$B$4*$B$7</f>
-        <v>603.14401887331815</v>
+        <f t="shared" si="5"/>
+        <v>753.93002359164757</v>
       </c>
       <c r="K17">
-        <f>J17/I17</f>
-        <v>3.2192378698224848</v>
+        <f t="shared" si="6"/>
+        <v>4.0240473372781054</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -954,40 +971,40 @@
         <v>0.81200000000000006</v>
       </c>
       <c r="C18">
-        <f>(PI()*(B18/1000/2)^2)</f>
+        <f t="shared" si="0"/>
         <v>5.1784756664712714E-7</v>
       </c>
       <c r="D18">
-        <f>B18/1000*$B$8*PI()</f>
+        <f t="shared" si="1"/>
         <v>3.0611678816578943E-3</v>
       </c>
       <c r="E18">
-        <f>C18*$B$8</f>
+        <f t="shared" si="2"/>
         <v>6.2141707997655255E-7</v>
       </c>
       <c r="F18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>5.2199034718030416E-3</v>
       </c>
       <c r="G18" s="3">
-        <f>($B$2*1)/C18</f>
+        <f t="shared" si="8"/>
         <v>2.1241772113019595</v>
       </c>
       <c r="H18">
-        <f>$B$9/(G18*$B$8)</f>
+        <f t="shared" si="3"/>
         <v>7.6500208709234689</v>
       </c>
       <c r="I18">
-        <f>H18*$B$9</f>
+        <f t="shared" si="4"/>
         <v>149.17540698300763</v>
       </c>
       <c r="J18">
-        <f>F18*$B$4*$B$7</f>
-        <v>480.23111940587978</v>
+        <f t="shared" si="5"/>
+        <v>600.28889925734973</v>
       </c>
       <c r="K18">
-        <f>J18/I18</f>
-        <v>3.2192378698224853</v>
+        <f t="shared" si="6"/>
+        <v>4.0240473372781063</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -998,40 +1015,40 @@
         <v>0.72</v>
       </c>
       <c r="C19">
-        <f>(PI()*(B19/1000/2)^2)</f>
+        <f t="shared" si="0"/>
         <v>4.0715040790523712E-7</v>
       </c>
       <c r="D19">
-        <f>B19/1000*$B$8*PI()</f>
+        <f t="shared" si="1"/>
         <v>2.7143360527015809E-3</v>
       </c>
       <c r="E19">
-        <f>C19*$B$8</f>
+        <f t="shared" si="2"/>
         <v>4.885804894862845E-7</v>
       </c>
       <c r="F19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>4.1040761116847898E-3</v>
       </c>
       <c r="G19" s="3">
-        <f>($B$2*1)/C19</f>
+        <f t="shared" si="8"/>
         <v>2.7017042808809402</v>
       </c>
       <c r="H19">
-        <f>$B$9/(G19*$B$8)</f>
+        <f t="shared" si="3"/>
         <v>6.0147219349637302</v>
       </c>
       <c r="I19">
-        <f>H19*$B$9</f>
+        <f t="shared" si="4"/>
         <v>117.28707773179273</v>
       </c>
       <c r="J19">
-        <f>F19*$B$4*$B$7</f>
-        <v>377.57500227500066</v>
+        <f t="shared" si="5"/>
+        <v>471.96875284375085</v>
       </c>
       <c r="K19">
-        <f>J19/I19</f>
-        <v>3.2192378698224848</v>
+        <f t="shared" si="6"/>
+        <v>4.0240473372781063</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1042,40 +1059,40 @@
         <v>0.64400000000000002</v>
       </c>
       <c r="C20">
-        <f>(PI()*(B20/1000/2)^2)</f>
+        <f t="shared" si="0"/>
         <v>3.2573289269480419E-7</v>
       </c>
       <c r="D20">
-        <f>B20/1000*$B$8*PI()</f>
+        <f t="shared" si="1"/>
         <v>2.4278228026941924E-3</v>
       </c>
       <c r="E20">
-        <f>C20*$B$8</f>
+        <f t="shared" si="2"/>
         <v>3.90879471233765E-7</v>
       </c>
       <c r="F20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>3.2833875583636262E-3</v>
       </c>
       <c r="G20" s="3">
-        <f>($B$2*1)/C20</f>
+        <f t="shared" si="8"/>
         <v>3.3770000656048156</v>
       </c>
       <c r="H20">
-        <f>$B$9/(G20*$B$8)</f>
+        <f t="shared" si="3"/>
         <v>4.8119631875368798</v>
       </c>
       <c r="I20">
-        <f>H20*$B$9</f>
+        <f t="shared" si="4"/>
         <v>93.833282156969162</v>
       </c>
       <c r="J20">
-        <f>F20*$B$4*$B$7</f>
-        <v>302.07165536945359</v>
+        <f t="shared" si="5"/>
+        <v>377.58956921181704</v>
       </c>
       <c r="K20">
-        <f>J20/I20</f>
-        <v>3.2192378698224848</v>
+        <f t="shared" si="6"/>
+        <v>4.0240473372781063</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1086,84 +1103,84 @@
         <v>0.57399999999999995</v>
       </c>
       <c r="C21">
-        <f>(PI()*(B21/1000/2)^2)</f>
+        <f t="shared" si="0"/>
         <v>2.5876984528353761E-7</v>
       </c>
       <c r="D21">
-        <f>B21/1000*$B$8*PI()</f>
+        <f t="shared" si="1"/>
         <v>2.1639290197926495E-3</v>
       </c>
       <c r="E21">
-        <f>C21*$B$8</f>
+        <f t="shared" si="2"/>
         <v>3.1052381434024511E-7</v>
       </c>
       <c r="F21">
+        <f t="shared" si="7"/>
+        <v>2.6084000404580591E-3</v>
+      </c>
+      <c r="G21" s="3">
+        <f t="shared" si="8"/>
+        <v>4.250881700666147</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="3"/>
+        <v>3.8227363507795324</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="4"/>
+        <v>74.543358840200881</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="5"/>
+        <v>299.96600465267682</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="6"/>
+        <v>4.0240473372781072</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>24</v>
+      </c>
+      <c r="B22" s="4">
+        <v>0.51100000000000001</v>
+      </c>
+      <c r="C22">
         <f t="shared" si="0"/>
-        <v>2.6084000404580591E-3</v>
-      </c>
-      <c r="G21" s="3">
-        <f>($B$2*1)/C21</f>
-        <v>4.250881700666147</v>
-      </c>
-      <c r="H21">
-        <f>$B$9/(G21*$B$8)</f>
-        <v>3.8227363507795324</v>
-      </c>
-      <c r="I21">
-        <f>H21*$B$9</f>
-        <v>74.543358840200881</v>
-      </c>
-      <c r="J21">
-        <f>F21*$B$4*$B$7</f>
-        <v>239.97280372214144</v>
-      </c>
-      <c r="K21">
-        <f>J21/I21</f>
-        <v>3.2192378698224857</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
-        <v>24</v>
-      </c>
-      <c r="B22" s="5">
-        <v>0.51100000000000001</v>
-      </c>
-      <c r="C22">
-        <f>(PI()*(B22/1000/2)^2)</f>
         <v>2.0508395382450515E-7</v>
       </c>
       <c r="D22">
-        <f>B22/1000*$B$8*PI()</f>
+        <f t="shared" si="1"/>
         <v>1.9264246151812613E-3</v>
       </c>
       <c r="E22">
-        <f>C22*$B$8</f>
+        <f t="shared" si="2"/>
         <v>2.4610074458940619E-7</v>
       </c>
       <c r="F22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>2.0672462545510122E-3</v>
       </c>
       <c r="G22" s="3">
-        <f>($B$2*1)/C22</f>
+        <f t="shared" si="8"/>
         <v>5.3636570754886765</v>
       </c>
       <c r="H22">
-        <f>$B$9/(G22*$B$8)</f>
+        <f t="shared" si="3"/>
         <v>3.0296493178620079</v>
       </c>
       <c r="I22">
-        <f>H22*$B$9</f>
+        <f t="shared" si="4"/>
         <v>59.078161698309152</v>
       </c>
       <c r="J22">
-        <f>F22*$B$4*$B$7</f>
-        <v>190.18665541869314</v>
+        <f t="shared" si="5"/>
+        <v>237.73331927336642</v>
       </c>
       <c r="K22">
-        <f>J22/I22</f>
-        <v>3.2192378698224862</v>
+        <f t="shared" si="6"/>
+        <v>4.0240473372781072</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1174,40 +1191,40 @@
         <v>0.45</v>
       </c>
       <c r="C23">
-        <f>(PI()*(B23/1000/2)^2)</f>
+        <f t="shared" si="0"/>
         <v>1.5904312808798326E-7</v>
       </c>
       <c r="D23">
-        <f>B23/1000*$B$8*PI()</f>
+        <f t="shared" si="1"/>
         <v>1.6964600329384882E-3</v>
       </c>
       <c r="E23">
-        <f>C23*$B$8</f>
+        <f t="shared" si="2"/>
         <v>1.908517537055799E-7</v>
       </c>
       <c r="F23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>1.6031547311268711E-3</v>
       </c>
       <c r="G23" s="3">
-        <f>($B$2*1)/C23</f>
+        <f t="shared" si="8"/>
         <v>6.9163629590552063</v>
       </c>
       <c r="H23">
-        <f>$B$9/(G23*$B$8)</f>
+        <f t="shared" si="3"/>
         <v>2.3495007558452072</v>
       </c>
       <c r="I23">
-        <f>H23*$B$9</f>
+        <f t="shared" si="4"/>
         <v>45.81526473898154</v>
       </c>
       <c r="J23">
-        <f>F23*$B$4*$B$7</f>
-        <v>147.49023526367216</v>
+        <f t="shared" si="5"/>
+        <v>184.3627940795902</v>
       </c>
       <c r="K23">
-        <f>J23/I23</f>
-        <v>3.2192378698224853</v>
+        <f t="shared" si="6"/>
+        <v>4.0240473372781072</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -1218,63 +1235,63 @@
         <v>0.40500000000000003</v>
       </c>
       <c r="C24">
-        <f>(PI()*(B24/1000/2)^2)</f>
+        <f t="shared" si="0"/>
         <v>1.2882493375126646E-7</v>
       </c>
       <c r="D24">
-        <f>B24/1000*$B$8*PI()</f>
+        <f t="shared" si="1"/>
         <v>1.5268140296446394E-3</v>
       </c>
       <c r="E24">
-        <f>C24*$B$8</f>
+        <f t="shared" si="2"/>
         <v>1.5458992050151975E-7</v>
       </c>
       <c r="F24">
+        <f t="shared" si="7"/>
+        <v>1.2985553322127658E-3</v>
+      </c>
+      <c r="G24" s="3">
+        <f t="shared" si="8"/>
+        <v>8.5387197025372892</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="3"/>
+        <v>1.9030956122346183</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="4"/>
+        <v>37.110364438575054</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="5"/>
+        <v>149.33386320446806</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="6"/>
+        <v>4.0240473372781063</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>27</v>
+      </c>
+      <c r="B25" s="5">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="C25">
         <f t="shared" si="0"/>
-        <v>1.2985553322127658E-3</v>
-      </c>
-      <c r="G24" s="3">
-        <f>($B$2*1)/C24</f>
-        <v>8.5387197025372892</v>
-      </c>
-      <c r="H24">
-        <f>$B$9/(G24*$B$8)</f>
-        <v>1.9030956122346183</v>
-      </c>
-      <c r="I24">
-        <f>H24*$B$9</f>
-        <v>37.110364438575054</v>
-      </c>
-      <c r="J24">
-        <f>F24*$B$4*$B$7</f>
-        <v>119.46709056357446</v>
-      </c>
-      <c r="K24">
-        <f>J24/I24</f>
-        <v>3.2192378698224848</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="7">
-        <v>27</v>
-      </c>
-      <c r="B25" s="7">
-        <v>0.36099999999999999</v>
-      </c>
-      <c r="C25">
-        <f>(PI()*(B25/1000/2)^2)</f>
         <v>1.0235387405211885E-7</v>
       </c>
       <c r="D25">
-        <f>B25/1000*$B$8*PI()</f>
+        <f t="shared" si="1"/>
         <v>1.3609379375350982E-3</v>
       </c>
       <c r="E25">
-        <f>C25*$B$8</f>
+        <f t="shared" si="2"/>
         <v>1.2282464886254261E-7</v>
       </c>
       <c r="F25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>1.0317270504453578E-3</v>
       </c>
       <c r="G25" s="3">
@@ -1282,7 +1299,7 @@
         <v>10.747028485115056</v>
       </c>
       <c r="H25">
-        <f>$B$9/(G25*$B$8)</f>
+        <f t="shared" si="3"/>
         <v>1.5120458666790284</v>
       </c>
       <c r="I25">
@@ -1290,12 +1307,12 @@
         <v>29.484894400241053</v>
       </c>
       <c r="J25">
-        <f>F25*$B$4*$B$7</f>
-        <v>94.918888640972924</v>
+        <f t="shared" si="5"/>
+        <v>118.64861080121615</v>
       </c>
       <c r="K25">
-        <f>J25/I25</f>
-        <v>3.2192378698224848</v>
+        <f t="shared" si="6"/>
+        <v>4.0240473372781063</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -1306,19 +1323,19 @@
         <v>0.32100000000000001</v>
       </c>
       <c r="C26">
-        <f>(PI()*(B26/1000/2)^2)</f>
+        <f t="shared" si="0"/>
         <v>8.0928212154636475E-8</v>
       </c>
       <c r="D26">
-        <f>B26/1000*$B$8*PI()</f>
+        <f t="shared" si="1"/>
         <v>1.2101414901627883E-3</v>
       </c>
       <c r="E26">
-        <f>C26*$B$8</f>
+        <f t="shared" si="2"/>
         <v>9.7113854585563768E-8</v>
       </c>
       <c r="F26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>8.1575637851873562E-4</v>
       </c>
       <c r="G26" s="3">
@@ -1326,20 +1343,20 @@
         <v>13.592293351274531</v>
       </c>
       <c r="H26">
-        <f>$B$9/(G26*$B$8)</f>
+        <f t="shared" si="3"/>
         <v>1.1955304068298571</v>
       </c>
       <c r="I26">
-        <f>H26*$B$9</f>
+        <f t="shared" si="4"/>
         <v>23.312842933182214</v>
       </c>
       <c r="J26">
-        <f>F26*$B$4*$B$7</f>
-        <v>75.049586823723686</v>
+        <f t="shared" si="5"/>
+        <v>93.811983529654597</v>
       </c>
       <c r="K26">
-        <f>J26/I26</f>
-        <v>3.2192378698224853</v>
+        <f t="shared" si="6"/>
+        <v>4.0240473372781063</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -1350,19 +1367,19 @@
         <v>0.28499999999999998</v>
       </c>
       <c r="C27">
-        <f>(PI()*(B27/1000/2)^2)</f>
+        <f t="shared" si="0"/>
         <v>6.3793965821957729E-8</v>
       </c>
       <c r="D27">
-        <f>B27/1000*$B$8*PI()</f>
+        <f t="shared" si="1"/>
         <v>1.0744246875277091E-3</v>
       </c>
       <c r="E27">
-        <f>C27*$B$8</f>
+        <f t="shared" si="2"/>
         <v>7.6552758986349267E-8</v>
       </c>
       <c r="F27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>6.4304317548533388E-4</v>
       </c>
       <c r="G27" s="3">
@@ -1370,20 +1387,20 @@
         <v>17.243010147229047</v>
       </c>
       <c r="H27">
-        <f>$B$9/(G27*$B$8)</f>
+        <f t="shared" si="3"/>
         <v>0.94241085873346642</v>
       </c>
       <c r="I27">
-        <f>H27*$B$9</f>
+        <f t="shared" si="4"/>
         <v>18.377011745302596</v>
       </c>
       <c r="J27">
-        <f>F27*$B$4*$B$7</f>
-        <v>59.159972144650716</v>
+        <f t="shared" si="5"/>
+        <v>73.949965180813393</v>
       </c>
       <c r="K27">
-        <f>J27/I27</f>
-        <v>3.2192378698224848</v>
+        <f t="shared" si="6"/>
+        <v>4.0240473372781063</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -1394,19 +1411,19 @@
         <v>0.255</v>
       </c>
       <c r="C28">
-        <f>(PI()*(B28/1000/2)^2)</f>
+        <f t="shared" si="0"/>
         <v>5.1070515574919089E-8</v>
       </c>
       <c r="D28">
-        <f>B28/1000*$B$8*PI()</f>
+        <f t="shared" si="1"/>
         <v>9.6132735199847669E-4</v>
       </c>
       <c r="E28">
-        <f>C28*$B$8</f>
+        <f t="shared" si="2"/>
         <v>6.1284618689902909E-8</v>
       </c>
       <c r="F28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>5.1479079699518447E-4</v>
       </c>
       <c r="G28" s="3">
@@ -1414,24 +1431,34 @@
         <v>21.538846585293022</v>
       </c>
       <c r="H28">
-        <f>$B$9/(G28*$B$8)</f>
+        <f t="shared" si="3"/>
         <v>0.75445079826585015</v>
       </c>
       <c r="I28">
-        <f>H28*$B$9</f>
+        <f t="shared" si="4"/>
         <v>14.711790566184078</v>
       </c>
       <c r="J28">
-        <f>F28*$B$4*$B$7</f>
-        <v>47.36075332355697</v>
+        <f t="shared" si="5"/>
+        <v>59.200941654446211</v>
       </c>
       <c r="K28">
-        <f>J28/I28</f>
-        <v>3.2192378698224857</v>
+        <f t="shared" si="6"/>
+        <v>4.0240473372781072</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="A68" s="8" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1442,8 +1469,11 @@
     <mergeCell ref="F2:K8"/>
     <mergeCell ref="G14:I14"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A68" r:id="rId1" xr:uid="{0EE0D02A-2CEA-447F-B91C-5B161459023D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>